<commit_message>
Added script 'plot_corrplot' to create a correlation matrix plot between all features in dataset
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/training_2016_2017_test_2018_2019_comparing_old_model/Q_river_Class_splitted/CK_Q_RIVER_CLASS_SPLIT.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/training_2016_2017_test_2018_2019_comparing_old_model/Q_river_Class_splitted/CK_Q_RIVER_CLASS_SPLIT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_Estuarine Box Model\Experiments\Parameters-Estimation\Ck_Parameters_Estimation\0-Dataset\training_2016_2017_test_2018_2019_comparing_old_model\Q_river_Class_splitted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE2239A-44E0-4E40-830E-FF7012F6C8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC40632-663C-4D87-9337-DBF60BAB9AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="5880" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,22 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Q_river</t>
+    <t>Qriver</t>
   </si>
   <si>
-    <t>Q_tide</t>
+    <t>Qtide</t>
   </si>
   <si>
-    <t>S_ocean</t>
+    <t>Socean</t>
   </si>
   <si>
-    <t>Ck_Obs</t>
+    <t>CkObs</t>
   </si>
   <si>
-    <t xml:space="preserve">Ck_Old_model </t>
+    <t xml:space="preserve">CkOldmodel </t>
   </si>
   <si>
-    <t>Q_river_class</t>
+    <t>QriverClass</t>
   </si>
 </sst>
 </file>
@@ -403,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1458" workbookViewId="0">
-      <selection activeCell="B1465" sqref="B1465"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added script to run ck experiment with Qriver class - added 'run_experiment_q_river_split_training_2016_2017_test_2018_2019' to run ck experiment both for low and strong qriver class
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/training_2016_2017_test_2018_2019_comparing_old_model/Q_river_Class_splitted/CK_Q_RIVER_CLASS_SPLIT.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/0-Dataset/training_2016_2017_test_2018_2019_comparing_old_model/Q_river_Class_splitted/CK_Q_RIVER_CLASS_SPLIT.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_Estuarine Box Model\Experiments\Parameters-Estimation\Ck_Parameters_Estimation\0-Dataset\training_2016_2017_test_2018_2019_comparing_old_model\Q_river_Class_splitted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC40632-663C-4D87-9337-DBF60BAB9AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CFF4A3-8ECC-4286-BAEA-8F798B5CCD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="5880" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4455" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ck_Q_river_splitted" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>